<commit_message>
added B24 services, API, Adapter and config
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -440,33 +440,33 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>440.00</t>
+          <t>660.00</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>660.00</t>
+          <t>440.00</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>60.00</t>
+          <t>1980.00</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -476,11 +476,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>190.00</t>
+          <t>880.00</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -496,27 +496,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2640.00</t>
+          <t>60.00</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>300.00</t>
+          <t>270.00</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>340.00</t>
+          <t>180.00</t>
         </is>
       </c>
       <c r="B10" t="n">

</xml_diff>

<commit_message>
feat(added default fields for statistic deal )
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,7 +440,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3">
@@ -450,57 +450,87 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1320.00</t>
+          <t>320.00</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>120.00</t>
+          <t>178.71</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>660.00</t>
+          <t>1320.00</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>880.00</t>
+          <t>660.00</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>270.00</t>
+          <t>120.00</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>300.00</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2640.00</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1100.00</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>